<commit_message>
SMTP Mail Sending from Private Domain
</commit_message>
<xml_diff>
--- a/employee.xlsx
+++ b/employee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patol\OneDrive\Desktop\Movya\BdayFestivalWishes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11727365-D776-488E-BA94-2769C216B62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B14678-CD34-4AA1-B1B6-DF8295D7F1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,15 +46,9 @@
     <t>Cobby Jackett</t>
   </si>
   <si>
-    <t>cjackett1@taobao.com</t>
-  </si>
-  <si>
     <t>Willette Pardie</t>
   </si>
   <si>
-    <t>wpardie2@rediff.com</t>
-  </si>
-  <si>
     <t>Divyesh Godhani</t>
   </si>
   <si>
@@ -65,6 +59,12 @@
   </si>
   <si>
     <t>abhi@movya.com</t>
+  </si>
+  <si>
+    <t>infinitelooprogramming@gmail.com</t>
+  </si>
+  <si>
+    <t>patoliyabhi17@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -483,11 +483,11 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="1">
-        <v>37638</v>
+        <v>45531</v>
       </c>
       <c r="E3" s="1">
         <v>45525</v>
@@ -498,16 +498,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>45525</v>
       </c>
       <c r="E4" s="1">
-        <v>45506</v>
+        <v>45531</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -515,10 +515,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1">
         <v>45525</v>
@@ -532,10 +532,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
         <v>45525</v>
@@ -548,6 +548,7 @@
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{A1AD44FD-84AC-488C-82F0-D1A8C31DCBA2}"/>
     <hyperlink ref="C6" r:id="rId2" xr:uid="{3AEE8366-2419-404E-A4F8-37E74886E8D1}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{EB15F61F-E430-4AAA-B31A-A17F315C473C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>